<commit_message>
Final pass before RLHub
</commit_message>
<xml_diff>
--- a/rlbase-data/rlbase_catalog.xlsx
+++ b/rlbase-data/rlbase_catalog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mille\Box Sync\Henry_Miller\Projects\RLoops_General\RMapDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CA7D7A-2D73-437D-9FD2-15F36BD9C089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE308AA0-0988-4E07-B74D-FD5ED3BC3B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9718" uniqueCount="1798">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9716" uniqueCount="1798">
   <si>
     <t>NT2</t>
   </si>
@@ -43004,10 +43004,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E69E83AD-33E0-472E-9601-5BFF6B08EDAB}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43019,16 +43019,6 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1784</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1237</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>